<commit_message>
Fixed Environment issues in Variable Light Env
</commit_message>
<xml_diff>
--- a/Intersections as Time Steps/Results/results.xlsx
+++ b/Intersections as Time Steps/Results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bking\Documents\Uni\Research\Thesis\Simulations\Intersections as Time Steps\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140B8E97-62FD-4BA3-849D-CEA93F66C09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6C38B9-1E5A-4594-BBBE-A6134C3FB986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12315" windowWidth="29040" windowHeight="16440" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="599" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="Table for PHEMlight V3" sheetId="10" r:id="rId7"/>
     <sheet name="Instructions" sheetId="3" r:id="rId8"/>
     <sheet name="new stuff" sheetId="11" r:id="rId9"/>
+    <sheet name="IT OVERFIT " sheetId="12" r:id="rId10"/>
+    <sheet name="Piecewise-Fcn" sheetId="13" r:id="rId11"/>
+    <sheet name="Env Issues" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
   <si>
     <t>Base</t>
   </si>
@@ -189,12 +192,129 @@
   <si>
     <t>model-velocity_based_30000.h5</t>
   </si>
+  <si>
+    <t>2nd training for 30000 on lab 3040</t>
+  </si>
+  <si>
+    <t>NOT BETTER THAN BASELINE</t>
+  </si>
+  <si>
+    <t>Previous tabs show the agent learning. However, it was overfitting to the scenarios I gave it.</t>
+  </si>
+  <si>
+    <t>I had screwed up the light phase observation, so it was only receiving information for the 9th traffic light</t>
+  </si>
+  <si>
+    <t>However, it still learned which speeds statistically were best to drive based on the distance between intersections</t>
+  </si>
+  <si>
+    <t>Therefore, it didn't matter the next state of the light, because it new if it saw distance "x", it would make it through the light "p%" of the time if it drove a specific speed</t>
+  </si>
+  <si>
+    <t>Here a training plot when I removed the phase observation altogether and it is very similar to the plots in previous tabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Here is a plot from one of the previous trainings… the phase observation was trash </t>
+  </si>
+  <si>
+    <t>With the correct phase observation included, it doesn't appear much has changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Variable light times, and trained without light times as an obs. It learns to command 20m/s always (correct decision given the environment and given obs). </t>
+  </si>
+  <si>
+    <t>average of 53</t>
+  </si>
+  <si>
+    <t>baseline of 56</t>
+  </si>
+  <si>
+    <t>Rewarding 1 for driving 15 and 25</t>
+  </si>
+  <si>
+    <t>Penalize outside of this band (-2 reward)</t>
+  </si>
+  <si>
+    <t>Penalize -1 for going under 1</t>
+  </si>
+  <si>
+    <t>Average fuel consumption: 52.14613670441933</t>
+  </si>
+  <si>
+    <t>Baseline around 56</t>
+  </si>
+  <si>
+    <t>Conclusion:</t>
+  </si>
+  <si>
+    <t>This may work but I never gave the car info on the original light phases</t>
+  </si>
+  <si>
+    <t>The obs are the velocity, the gap until the next interesection, the time until the next phase change, and the next phase. It doesn't need to know how long the other phase (red if green light and vice versa) because I contrained all light cycles to be exactly 60 seconds)... UPDATE: it does need to know the length of at least one phase which I didn't give it. I was only giving it time until light changed here which isn't enough info. It was learning to exploit the average distances and light times instead of using phase info)</t>
+  </si>
+  <si>
+    <t>why did it fail</t>
+  </si>
+  <si>
+    <t>Retraining because of issues with the environment</t>
+  </si>
+  <si>
+    <t>One of the light states was not working</t>
+  </si>
+  <si>
+    <t>Every reset, the observation would be [0,0,0,0] which may have been messing with training as it took place every episode and gave the model no valuable action-reward knowledge</t>
+  </si>
+  <si>
+    <t>To remedy, now the vehicle is automatically sent back to the beginning without terminating the episode if it reaches the  8th light</t>
+  </si>
+  <si>
+    <t>The car would terminate at a time (400 seconds). It was probably counting the terminating state as a 0 value state and therefore tried to avoid it in the future</t>
+  </si>
+  <si>
+    <t>This was fixed by adding an extra vehicle movement at every reset()</t>
+  </si>
+  <si>
+    <t>Episode vs reward plot</t>
+  </si>
+  <si>
+    <t>Moving average of plot on left</t>
+  </si>
+  <si>
+    <t>Sample runs after training</t>
+  </si>
+  <si>
+    <t>Reward function</t>
+  </si>
+  <si>
+    <t>1 between 10 and 30</t>
+  </si>
+  <si>
+    <t>minus .5 outside of this band</t>
+  </si>
+  <si>
+    <t>minus 1 for stopping</t>
+  </si>
+  <si>
+    <t>These results could just be due to the decreasing epsilon value</t>
+  </si>
+  <si>
+    <t>baseline around 57 mL/meter</t>
+  </si>
+  <si>
+    <t>average around 54 mL/meter which is better than baseline</t>
+  </si>
+  <si>
+    <t>improvement</t>
+  </si>
+  <si>
+    <t>trained and looking good but actually performed same as baseline (57 mL/m)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,8 +330,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,6 +354,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,10 +576,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -487,16 +627,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -22547,6 +22698,627 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>153832</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>56838</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26DDE212-7B9A-C9DD-4B6B-055B56BCA32F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="640080" y="2499360"/>
+          <a:ext cx="3780952" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>58609</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>121625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{969B2175-A3F0-6501-78E8-177FCEC51915}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5631180" y="2514600"/>
+          <a:ext cx="3571429" cy="2361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>18590</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BACA5C82-891F-605F-76D8-5DCB43A95CF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="2560320"/>
+          <a:ext cx="3676190" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>590095</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E49DAB0-86E6-940C-B703-BB5D5F3375D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="5120640"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>590095</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D83C8F7-E2BD-B517-CC87-2251ED484ABB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="7863840"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>590095</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA0A966C-0244-041A-A63E-945E975BB0A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="10607040"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>56695</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>26358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{394C1C98-A099-2493-137E-2A9DB1BD5E76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10439400" y="13258800"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>43369</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>83525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2113E4BA-10CF-DC6C-31C6-DE258CDB86F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5615940" y="6316980"/>
+          <a:ext cx="3571429" cy="2361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9062</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>26358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E1B38C3-1F98-D88B-CBE2-7AF4C8CC7359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5448300" y="9784080"/>
+          <a:ext cx="3704762" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>75733</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E53F212-9650-6A5E-AE08-C9E7B121C592}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="12070080"/>
+          <a:ext cx="3733333" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>590095</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA942576-BD27-0613-0E69-0BF63751CDC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="14813280"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>75733</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDCCD59F-029D-A0C2-56FD-CA0B9F12B736}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="17556480"/>
+          <a:ext cx="3733333" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>89089</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>144485</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FF0B9EC-322A-ACD7-8896-DCE45F8FC39B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6271260" y="20825460"/>
+          <a:ext cx="3571429" cy="2361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>350034</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>87318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC8312D-A271-0844-AB10-12D07E84C044}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="731520" y="20817840"/>
+          <a:ext cx="3885714" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -23769,6 +24541,500 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>230032</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>148278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D01CF313-DA27-FAAF-D850-6D276A82B110}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="2042160"/>
+          <a:ext cx="3780952" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>45721</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>205741</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>157271</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D448344B-D0B1-1889-4B13-18899F03F97F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6797041" y="2156460"/>
+          <a:ext cx="3208020" cy="2024171"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>397672</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>56838</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{222F4AE0-F374-8C84-EC47-577CD1066C25}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="929640" y="5425440"/>
+          <a:ext cx="3780952" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342433</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>94938</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF345845-6A9D-9306-3EFD-86A6E6488A49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531620" y="12778740"/>
+          <a:ext cx="3733333" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>590095</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE6146E5-BC2D-C15F-B6BD-89DEE5DD36F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7360920" y="12801600"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>605335</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>148278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE4AECB9-AF72-F948-700F-DBEBDA2B0369}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7376160" y="15392400"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>128005</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26C8B39B-1DB0-5949-828E-8EFBF347DD06}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7658100" y="10416540"/>
+          <a:ext cx="3253740" cy="2147305"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>393855</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>3498</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A773F464-CF21-6A84-4976-31F72AC842F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1478280" y="9944100"/>
+          <a:ext cx="3838095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>123352</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92108516-8BA3-02FD-4A19-F9814D142D6B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7360920" y="18288000"/>
+          <a:ext cx="3780952" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123352</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>117798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF87F29B-B5A3-DC84-1691-15427483D1CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="914400"/>
+          <a:ext cx="3780952" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>18576</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>72078</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53EBDC85-4584-C559-2A6E-94B64D624A05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7810500" y="868680"/>
+          <a:ext cx="3790476" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -24053,15 +25319,15 @@
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="37"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="2"/>
       <c r="J3" s="16" t="s">
         <v>10</v>
@@ -24069,15 +25335,15 @@
     </row>
     <row r="4" spans="2:10" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="41"/>
       <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
@@ -24362,7 +25628,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16 D16">
+  <conditionalFormatting sqref="D16 G16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -24376,6 +25642,998 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42A8A10-872E-4969-A1E7-59F7FE8D99C1}">
+  <dimension ref="A1:V117"/>
+  <sheetViews>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="U66" sqref="U66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="37">
+        <v>44953</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="K10" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B11" s="43"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="38"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B35" s="38"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+    </row>
+    <row r="47" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="36"/>
+      <c r="P47" s="36"/>
+      <c r="Q47" s="36"/>
+      <c r="R47" s="36"/>
+      <c r="S47" s="36"/>
+      <c r="T47" s="36"/>
+      <c r="U47" s="36"/>
+      <c r="V47" s="36"/>
+    </row>
+    <row r="51" spans="3:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
+      <c r="L51" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="M51" s="44"/>
+      <c r="N51" s="44"/>
+      <c r="O51" s="44"/>
+      <c r="P51" s="44"/>
+      <c r="Q51" s="44"/>
+      <c r="R51" s="44"/>
+      <c r="S51" s="44"/>
+    </row>
+    <row r="52" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C52" s="44"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="44"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="44"/>
+      <c r="N52" s="44"/>
+      <c r="O52" s="44"/>
+      <c r="P52" s="44"/>
+      <c r="Q52" s="44"/>
+      <c r="R52" s="44"/>
+      <c r="S52" s="44"/>
+    </row>
+    <row r="53" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C53" s="44"/>
+      <c r="D53" s="44"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="L53" s="44"/>
+      <c r="M53" s="44"/>
+      <c r="N53" s="44"/>
+      <c r="O53" s="44"/>
+      <c r="P53" s="44"/>
+      <c r="Q53" s="44"/>
+      <c r="R53" s="44"/>
+      <c r="S53" s="44"/>
+    </row>
+    <row r="54" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="44"/>
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="L54" s="44"/>
+      <c r="M54" s="44"/>
+      <c r="N54" s="44"/>
+      <c r="O54" s="44"/>
+      <c r="P54" s="44"/>
+      <c r="Q54" s="44"/>
+      <c r="R54" s="44"/>
+      <c r="S54" s="44"/>
+    </row>
+    <row r="55" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="39"/>
+      <c r="I55" s="39"/>
+      <c r="L55" s="44"/>
+      <c r="M55" s="44"/>
+      <c r="N55" s="44"/>
+      <c r="O55" s="44"/>
+      <c r="P55" s="44"/>
+      <c r="Q55" s="44"/>
+      <c r="R55" s="44"/>
+      <c r="S55" s="44"/>
+    </row>
+    <row r="56" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
+      <c r="H56" s="39"/>
+      <c r="I56" s="39"/>
+      <c r="L56" s="44"/>
+      <c r="M56" s="44"/>
+      <c r="N56" s="44"/>
+      <c r="O56" s="44"/>
+      <c r="P56" s="44"/>
+      <c r="Q56" s="44"/>
+      <c r="R56" s="44"/>
+      <c r="S56" s="44"/>
+    </row>
+    <row r="57" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="39"/>
+      <c r="H57" s="39"/>
+      <c r="I57" s="39"/>
+      <c r="L57" s="44"/>
+      <c r="M57" s="44"/>
+      <c r="N57" s="44"/>
+      <c r="O57" s="44"/>
+      <c r="P57" s="44"/>
+      <c r="Q57" s="44"/>
+      <c r="R57" s="44"/>
+      <c r="S57" s="44"/>
+    </row>
+    <row r="58" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="L58" s="39"/>
+      <c r="M58" s="39"/>
+      <c r="N58" s="39"/>
+      <c r="O58" s="39"/>
+      <c r="P58" s="39"/>
+      <c r="Q58" s="39"/>
+      <c r="R58" s="39"/>
+      <c r="S58" s="39"/>
+    </row>
+    <row r="59" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="39"/>
+      <c r="H59" s="39"/>
+      <c r="I59" s="39"/>
+      <c r="L59" s="39"/>
+      <c r="M59" s="39"/>
+      <c r="N59" s="39"/>
+      <c r="O59" s="39"/>
+      <c r="P59" s="39"/>
+      <c r="Q59" s="39"/>
+      <c r="R59" s="39"/>
+      <c r="S59" s="39"/>
+    </row>
+    <row r="60" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C60" s="39"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="39"/>
+      <c r="O60" s="39"/>
+      <c r="P60" s="39"/>
+      <c r="Q60" s="39"/>
+      <c r="R60" s="39"/>
+      <c r="S60" s="39"/>
+    </row>
+    <row r="61" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="39"/>
+      <c r="L61" s="39"/>
+      <c r="M61" s="39"/>
+      <c r="N61" s="39"/>
+      <c r="O61" s="39"/>
+      <c r="P61" s="39"/>
+      <c r="Q61" s="39"/>
+      <c r="R61" s="39"/>
+      <c r="S61" s="39"/>
+    </row>
+    <row r="62" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="39"/>
+      <c r="L62" s="39"/>
+      <c r="M62" s="39"/>
+      <c r="N62" s="39"/>
+      <c r="O62" s="39"/>
+      <c r="P62" s="39"/>
+      <c r="Q62" s="39"/>
+      <c r="R62" s="39"/>
+      <c r="S62" s="39"/>
+    </row>
+    <row r="63" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C63" s="39"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="39"/>
+      <c r="H63" s="39"/>
+      <c r="I63" s="39"/>
+      <c r="L63" s="39"/>
+      <c r="M63" s="39"/>
+      <c r="N63" s="39"/>
+      <c r="O63" s="39"/>
+      <c r="P63" s="39"/>
+      <c r="Q63" s="39"/>
+      <c r="R63" s="39"/>
+      <c r="S63" s="39"/>
+    </row>
+    <row r="64" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="39"/>
+      <c r="H64" s="39"/>
+      <c r="I64" s="39"/>
+      <c r="L64" s="39"/>
+      <c r="M64" s="39"/>
+      <c r="N64" s="39"/>
+      <c r="O64" s="39"/>
+      <c r="P64" s="39"/>
+      <c r="Q64" s="39"/>
+      <c r="R64" s="39"/>
+      <c r="S64" s="39"/>
+    </row>
+    <row r="65" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C65" s="39"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="39"/>
+      <c r="H65" s="39"/>
+      <c r="I65" s="39"/>
+      <c r="L65" s="39"/>
+      <c r="M65" s="39"/>
+      <c r="N65" s="39"/>
+      <c r="O65" s="39"/>
+      <c r="P65" s="39"/>
+      <c r="Q65" s="39"/>
+      <c r="R65" s="39"/>
+      <c r="S65" s="39"/>
+    </row>
+    <row r="66" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C66" s="39"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="39"/>
+      <c r="H66" s="39"/>
+      <c r="I66" s="39"/>
+      <c r="L66" s="39"/>
+      <c r="M66" s="39"/>
+      <c r="N66" s="39"/>
+      <c r="O66" s="39"/>
+      <c r="P66" s="39"/>
+      <c r="Q66" s="39"/>
+      <c r="R66" s="39"/>
+      <c r="S66" s="39"/>
+    </row>
+    <row r="67" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C67" s="39"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="39"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="39"/>
+      <c r="L67" s="39"/>
+      <c r="M67" s="39"/>
+      <c r="N67" s="39"/>
+      <c r="O67" s="39"/>
+      <c r="P67" s="39"/>
+      <c r="Q67" s="39"/>
+      <c r="R67" s="39"/>
+      <c r="S67" s="39"/>
+    </row>
+    <row r="68" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="39"/>
+      <c r="L68" s="39"/>
+      <c r="M68" s="39"/>
+      <c r="N68" s="39"/>
+      <c r="O68" s="39"/>
+      <c r="P68" s="39"/>
+      <c r="Q68" s="39"/>
+      <c r="R68" s="39"/>
+      <c r="S68" s="39"/>
+    </row>
+    <row r="69" spans="3:19" x14ac:dyDescent="0.3">
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="39"/>
+      <c r="H69" s="39"/>
+      <c r="I69" s="39"/>
+      <c r="L69" s="39"/>
+      <c r="M69" s="39"/>
+      <c r="N69" s="39"/>
+      <c r="O69" s="39"/>
+      <c r="P69" s="39"/>
+      <c r="Q69" s="39"/>
+      <c r="R69" s="39"/>
+      <c r="S69" s="39"/>
+    </row>
+    <row r="116" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M116" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="117" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M117" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B10:H11"/>
+    <mergeCell ref="K10:Q11"/>
+    <mergeCell ref="B28:H29"/>
+    <mergeCell ref="C51:I54"/>
+    <mergeCell ref="L51:S57"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9ED441F-6E68-4C8F-9B81-7A11833A2CC4}">
+  <dimension ref="B2:N24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="N21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0534FAAE-C29B-43FB-9460-07F6A786BB0D}">
+  <dimension ref="B2:R130"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="K140" sqref="K139:K140"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" t="s">
+        <v>76</v>
+      </c>
+      <c r="R13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J52" t="s">
+        <v>85</v>
+      </c>
+      <c r="K52" s="40">
+        <f>(54-57)/57</f>
+        <v>-5.2631578947368418E-2</v>
+      </c>
+    </row>
+    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C130" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -40271,7 +42529,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B2:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -40289,15 +42547,15 @@
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="37"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="2"/>
       <c r="J3" s="16" t="s">
         <v>10</v>
@@ -40308,15 +42566,15 @@
     </row>
     <row r="4" spans="2:14" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="41"/>
       <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
@@ -40534,7 +42792,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16 G16">
+  <conditionalFormatting sqref="G16 D16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -40546,7 +42804,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16 J16 D16">
+  <conditionalFormatting sqref="J16 G16 D16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -40569,8 +42827,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:R404"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45533,8 +47791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B8EBAC-B352-4AAA-920D-03008C82BE3C}">
   <dimension ref="B2:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45555,15 +47813,15 @@
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="37"/>
+      <c r="H3" s="42"/>
       <c r="I3" s="2"/>
       <c r="J3" s="16" t="s">
         <v>10</v>
@@ -45574,15 +47832,15 @@
     </row>
     <row r="4" spans="2:14" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="36"/>
+      <c r="E4" s="41"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="36"/>
+      <c r="H4" s="41"/>
       <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
@@ -45800,7 +48058,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16 G16">
+  <conditionalFormatting sqref="G16 D16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -45812,7 +48070,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16 J16 D16">
+  <conditionalFormatting sqref="J16 G16 D16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -45914,17 +48172,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D12A82-B62F-42C4-8BAC-0205C77AF4B6}">
-  <dimension ref="B1:V33"/>
+  <dimension ref="B1:AR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="10" max="10" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.88671875" customWidth="1"/>
-    <col min="20" max="20" width="8.88671875" style="38"/>
+    <col min="20" max="20" width="8.88671875" style="36"/>
+    <col min="44" max="44" width="8.88671875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.3">
@@ -45937,17 +48196,22 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.3">
       <c r="L17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="X20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>41</v>
       </c>
@@ -45958,8 +48222,11 @@
       <c r="V21">
         <v>57.510848939149</v>
       </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="X21">
+        <v>58.88</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I22" s="31" t="s">
         <v>43</v>
       </c>
@@ -45967,8 +48234,11 @@
       <c r="V22">
         <v>53.321522987116303</v>
       </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="X22">
+        <v>56.88</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I23" s="31">
         <v>56.214728914704203</v>
       </c>
@@ -45976,8 +48246,11 @@
       <c r="V23">
         <v>69.810628879342104</v>
       </c>
-    </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="X23">
+        <v>56.83</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I24" s="31">
         <v>50.855851321865003</v>
       </c>
@@ -45987,8 +48260,11 @@
       <c r="V24">
         <v>82.913693645783894</v>
       </c>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="X24">
+        <v>59.22</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I25" s="31">
         <v>55.696652815891703</v>
       </c>
@@ -45996,8 +48272,11 @@
       <c r="V25">
         <v>55.268045832159302</v>
       </c>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="X25">
+        <v>53.16</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I26" s="31">
         <v>56.500208049264998</v>
       </c>
@@ -46007,8 +48286,11 @@
       <c r="V26">
         <v>55.474706010285203</v>
       </c>
-    </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="X26">
+        <v>58.83</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I27" s="31">
         <v>55.473038251193898</v>
       </c>
@@ -46017,7 +48299,7 @@
         <v>55.032721660596501</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I28" s="31">
         <v>52.853714812164498</v>
       </c>
@@ -46028,7 +48310,7 @@
         <v>56.306273233987397</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I29" s="31">
         <v>55.039542822277397</v>
       </c>
@@ -46037,7 +48319,7 @@
         <v>55.906917208049897</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I30" s="31">
         <v>53.087811550421598</v>
       </c>
@@ -46046,7 +48328,7 @@
         <v>55.804629373724502</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I31" s="31">
         <v>54.381807707836003</v>
       </c>
@@ -46055,11 +48337,14 @@
         <v>55.442090438280701</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.3">
       <c r="I32" s="34" t="s">
         <v>5</v>
       </c>
       <c r="J32" s="32"/>
+      <c r="X32" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="33" spans="9:22" x14ac:dyDescent="0.3">
       <c r="I33" s="35">

</xml_diff>

<commit_message>
Normalized rewards and fixed environment issues
</commit_message>
<xml_diff>
--- a/Intersections as Time Steps/Results/results.xlsx
+++ b/Intersections as Time Steps/Results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bking\Documents\Uni\Research\Thesis\Simulations\Intersections as Time Steps\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6C38B9-1E5A-4594-BBBE-A6134C3FB986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9599DDD7-1419-455B-8A37-9324B2EB6CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="599" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Base</t>
   </si>
@@ -308,6 +308,9 @@
   </si>
   <si>
     <t>trained and looking good but actually performed same as baseline (57 mL/m)</t>
+  </si>
+  <si>
+    <t>53.5 mL/m</t>
   </si>
 </sst>
 </file>
@@ -23316,6 +23319,270 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>365279</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>87318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{377F134B-196B-F29E-033D-97DABC8D8568}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="784860" y="24292560"/>
+          <a:ext cx="3847619" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>508189</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>152105</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9227CC5B-7C0D-9C3C-FB8D-93471F0779D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6080760" y="24307800"/>
+          <a:ext cx="3571429" cy="2361905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>430075</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>26358</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{791DEB62-437B-7C6B-6F6C-365BE759A3DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5935980" y="26791920"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>551995</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>125418</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC6CEC40-9996-E3D4-FD2B-BB95C0C69790}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6057900" y="29268420"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>161448</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>18738</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F6F041D-DD7C-E77B-69C3-95046CF1AC8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="31722060"/>
+          <a:ext cx="3819048" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>56695</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>133038</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF82347-016C-F7D2-4727-F5509A92587E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6172200" y="34213800"/>
+          <a:ext cx="3638095" cy="2495238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -25628,7 +25895,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16 G16">
+  <conditionalFormatting sqref="G16 D16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -26534,10 +26801,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0534FAAE-C29B-43FB-9460-07F6A786BB0D}">
-  <dimension ref="B2:R130"/>
+  <dimension ref="B2:R149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="K140" sqref="K139:K140"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="U186" sqref="U186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26629,6 +26896,11 @@
     <row r="130" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C149" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -42792,7 +43064,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16 D16">
+  <conditionalFormatting sqref="D16 G16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -42804,7 +43076,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16 G16 D16">
+  <conditionalFormatting sqref="G16 J16 D16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -48058,7 +48330,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G16 D16">
+  <conditionalFormatting sqref="D16 G16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -48070,7 +48342,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J16 G16 D16">
+  <conditionalFormatting sqref="G16 J16 D16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>